<commit_message>
Add end-to-end ML project notebook
Added 02_v2_end_to_end_machine_learning_project.ipynb containing sample code and solutions for an end-to-end machine learning project. Minor update to universal_registry_MASTER.xlsx.
</commit_message>
<xml_diff>
--- a/universal_registry_MASTER.xlsx
+++ b/universal_registry_MASTER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aresources\workspace\mac-py\mac-handson-ml3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E027642D-9780-431F-BB09-DC6355F290C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03A8920-F97F-420B-A8EA-D10095435D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registry" sheetId="1" r:id="rId1"/>
@@ -2961,7 +2961,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2976,11 +2976,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3526,7 +3521,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3542,7 +3537,7 @@
     <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="61" customWidth="1"/>
+    <col min="12" max="12" width="104.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="36.140625" bestFit="1" customWidth="1"/>
@@ -3608,27 +3603,27 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6">
         <v>3</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="8">
         <v>45968.835113136571</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="6" t="s">
         <v>21</v>
       </c>
       <c r="L2" t="s">
@@ -3654,29 +3649,29 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6">
         <v>4</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="8">
         <v>45968.835113159723</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="6" t="s">
         <v>21</v>
       </c>
       <c r="L3" t="s">
@@ -3702,27 +3697,27 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6">
         <v>4</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="8">
         <v>45968.835113159723</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="6" t="s">
         <v>21</v>
       </c>
       <c r="L4" t="s">
@@ -3748,31 +3743,31 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9">
+      <c r="E5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6">
         <v>7</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="8">
         <v>45968.835113194436</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="6" t="s">
         <v>21</v>
       </c>
       <c r="L5" t="s">
@@ -3798,29 +3793,29 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9">
+      <c r="E6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6">
         <v>3</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="8">
         <v>45968.835113217603</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="L6" t="s">
@@ -3846,29 +3841,29 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9">
-        <v>26</v>
-      </c>
-      <c r="J7" s="11">
+      <c r="E7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6">
+        <v>26</v>
+      </c>
+      <c r="J7" s="8">
         <v>45968.835113240741</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="6" t="s">
         <v>21</v>
       </c>
       <c r="L7" t="s">
@@ -3894,29 +3889,29 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9">
-        <v>26</v>
-      </c>
-      <c r="J8" s="11">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6">
+        <v>26</v>
+      </c>
+      <c r="J8" s="8">
         <v>45968.835113240741</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="6" t="s">
         <v>21</v>
       </c>
       <c r="L8" t="s">
@@ -3942,29 +3937,29 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6">
         <v>10</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="8">
         <v>45968.835113240741</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="6" t="s">
         <v>21</v>
       </c>
       <c r="L9" t="s">
@@ -3990,29 +3985,29 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6">
         <v>11</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="8">
         <v>45968.835113321758</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="6" t="s">
         <v>21</v>
       </c>
       <c r="L10" t="s">
@@ -4038,29 +4033,29 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9">
+      <c r="H11" s="6"/>
+      <c r="I11" s="6">
         <v>11</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="8">
         <v>45968.835113321758</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="6" t="s">
         <v>21</v>
       </c>
       <c r="L11" t="s">
@@ -4083,29 +4078,29 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6">
         <v>11</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="8">
         <v>45968.83511334491</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="6" t="s">
         <v>21</v>
       </c>
       <c r="L12" t="s">
@@ -4131,29 +4126,29 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6">
         <v>10</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="8">
         <v>45968.835113611109</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" s="6" t="s">
         <v>21</v>
       </c>
       <c r="L13" t="s">
@@ -4179,29 +4174,29 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6">
         <v>22</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="8">
         <v>45968.83511378472</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" s="6" t="s">
         <v>21</v>
       </c>
       <c r="L14" t="s">
@@ -4227,29 +4222,29 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9">
+      <c r="D15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6">
         <v>22</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="8">
         <v>45968.83511378472</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="6" t="s">
         <v>21</v>
       </c>
       <c r="L15" t="s">
@@ -4931,25 +4926,29 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="A31" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I31">
+      <c r="D31" s="6"/>
+      <c r="E31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6">
         <v>4</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J31" s="8">
         <v>45968.835115486108</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L31" t="s">
@@ -4975,22 +4974,27 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="A32" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E32" t="s">
-        <v>20</v>
-      </c>
-      <c r="I32">
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6">
         <v>4</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J32" s="8">
         <v>45968.835115486108</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K32" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L32" t="s">
@@ -5016,28 +5020,31 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="A33" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E33" t="s">
-        <v>20</v>
-      </c>
-      <c r="I33">
+      <c r="E33" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6">
         <v>1</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J33" s="8">
         <v>45968.835115520837</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K33" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L33" t="s">
@@ -5063,25 +5070,29 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="A34" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E34" t="s">
-        <v>20</v>
-      </c>
-      <c r="I34">
+      <c r="D34" s="6"/>
+      <c r="E34" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6">
         <v>16</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="8">
         <v>45968.835115520837</v>
       </c>
-      <c r="K34" t="s">
+      <c r="K34" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L34" t="s">
@@ -5107,25 +5118,29 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="A35" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D35" t="s">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E35" t="s">
-        <v>20</v>
-      </c>
-      <c r="I35">
+      <c r="E35" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="6"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6">
         <v>16</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J35" s="8">
         <v>45968.835115520837</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K35" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L35" t="s">
@@ -5151,22 +5166,27 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>18</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="A36" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E36" t="s">
-        <v>20</v>
-      </c>
-      <c r="I36">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="6"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6">
         <v>16</v>
       </c>
-      <c r="J36" s="2">
+      <c r="J36" s="8">
         <v>45968.835115520837</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K36" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L36" t="s">
@@ -5192,25 +5212,29 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="A37" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E37" t="s">
-        <v>20</v>
-      </c>
-      <c r="I37">
+      <c r="D37" s="6"/>
+      <c r="E37" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="6"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6">
         <v>16</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J37" s="8">
         <v>45968.835115520837</v>
       </c>
-      <c r="K37" t="s">
+      <c r="K37" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L37" t="s">
@@ -5236,22 +5260,27 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E38" t="s">
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I38">
+      <c r="G38" s="7"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6">
         <v>16</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J38" s="8">
         <v>45968.835115520837</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K38" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L38" t="s">
@@ -5274,25 +5303,29 @@
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E39" t="s">
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G39" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="I39">
+      <c r="H39" s="6"/>
+      <c r="I39" s="6">
         <v>10</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J39" s="8">
         <v>45968.835115671303</v>
       </c>
-      <c r="K39" t="s">
+      <c r="K39" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L39" t="s">
@@ -5315,25 +5348,29 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="A40" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D40" t="s">
+      <c r="C40" s="6"/>
+      <c r="D40" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E40" t="s">
-        <v>20</v>
-      </c>
-      <c r="I40">
+      <c r="E40" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="6"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6">
         <v>8</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J40" s="8">
         <v>45968.835115740738</v>
       </c>
-      <c r="K40" t="s">
+      <c r="K40" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L40" t="s">
@@ -5359,25 +5396,29 @@
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E41" t="s">
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="G41" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I41">
+      <c r="H41" s="6"/>
+      <c r="I41" s="6">
         <v>8</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J41" s="8">
         <v>45968.835115740738</v>
       </c>
-      <c r="K41" t="s">
+      <c r="K41" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L41" t="s">
@@ -5400,25 +5441,29 @@
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>18</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="A42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E42" t="s">
-        <v>20</v>
-      </c>
-      <c r="I42">
+      <c r="D42" s="6"/>
+      <c r="E42" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="6"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6">
         <v>9</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J42" s="8">
         <v>45968.835115787027</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K42" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L42" t="s">
@@ -5444,25 +5489,29 @@
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E43" t="s">
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="G43" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="I43">
+      <c r="H43" s="6"/>
+      <c r="I43" s="6">
         <v>9</v>
       </c>
-      <c r="J43" s="2">
+      <c r="J43" s="8">
         <v>45968.835115787027</v>
       </c>
-      <c r="K43" t="s">
+      <c r="K43" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L43" t="s">
@@ -5485,25 +5534,29 @@
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E44" t="s">
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="G44" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I44">
+      <c r="H44" s="6"/>
+      <c r="I44" s="6">
         <v>9</v>
       </c>
-      <c r="J44" s="2">
+      <c r="J44" s="8">
         <v>45968.835115787027</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K44" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L44" t="s">
@@ -5526,25 +5579,29 @@
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>18</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="A45" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E45" t="s">
-        <v>20</v>
-      </c>
-      <c r="I45">
+      <c r="D45" s="6"/>
+      <c r="E45" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="6"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6">
         <v>3</v>
       </c>
-      <c r="J45" s="2">
+      <c r="J45" s="8">
         <v>45968.835115902781</v>
       </c>
-      <c r="K45" t="s">
+      <c r="K45" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L45" t="s">
@@ -5570,25 +5627,29 @@
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>18</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="A46" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I46">
+      <c r="D46" s="6"/>
+      <c r="E46" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="6"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6">
         <v>9</v>
       </c>
-      <c r="J46" s="2">
+      <c r="J46" s="8">
         <v>45968.835115960646</v>
       </c>
-      <c r="K46" t="s">
+      <c r="K46" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L46" t="s">
@@ -5614,25 +5675,29 @@
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>18</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="A47" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E47" t="s">
-        <v>20</v>
-      </c>
-      <c r="I47">
+      <c r="D47" s="6"/>
+      <c r="E47" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="6"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6">
         <v>8</v>
       </c>
-      <c r="J47" s="2">
+      <c r="J47" s="8">
         <v>45968.835116041657</v>
       </c>
-      <c r="K47" t="s">
+      <c r="K47" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L47" t="s">
@@ -5658,25 +5723,29 @@
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E48" t="s">
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G48" s="3" t="s">
+      <c r="G48" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="I48">
-        <v>18</v>
-      </c>
-      <c r="J48" s="2">
+      <c r="H48" s="6"/>
+      <c r="I48" s="6">
+        <v>18</v>
+      </c>
+      <c r="J48" s="8">
         <v>45968.835116122682</v>
       </c>
-      <c r="K48" t="s">
+      <c r="K48" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L48" t="s">
@@ -5699,25 +5768,29 @@
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>18</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="A49" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E49" t="s">
-        <v>20</v>
-      </c>
-      <c r="I49">
+      <c r="D49" s="6"/>
+      <c r="E49" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" s="6"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6">
         <v>7</v>
       </c>
-      <c r="J49" s="2">
+      <c r="J49" s="8">
         <v>45968.835116319453</v>
       </c>
-      <c r="K49" t="s">
+      <c r="K49" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L49" t="s">
@@ -5743,25 +5816,29 @@
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>18</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="A50" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E50" t="s">
-        <v>20</v>
-      </c>
-      <c r="I50">
+      <c r="D50" s="6"/>
+      <c r="E50" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" s="6"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6">
         <v>3</v>
       </c>
-      <c r="J50" s="2">
+      <c r="J50" s="8">
         <v>45968.835116481481</v>
       </c>
-      <c r="K50" t="s">
+      <c r="K50" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L50" t="s">
@@ -5787,25 +5864,29 @@
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="A51" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E51" t="s">
-        <v>20</v>
-      </c>
-      <c r="I51">
+      <c r="D51" s="6"/>
+      <c r="E51" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" s="6"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6">
         <v>4</v>
       </c>
-      <c r="J51" s="2">
+      <c r="J51" s="8">
         <v>45968.835116712973</v>
       </c>
-      <c r="K51" t="s">
+      <c r="K51" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L51" t="s">
@@ -5831,25 +5912,29 @@
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>18</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="A52" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E52" t="s">
-        <v>20</v>
-      </c>
-      <c r="I52">
+      <c r="D52" s="6"/>
+      <c r="E52" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="6"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6">
         <v>4</v>
       </c>
-      <c r="J52" s="2">
+      <c r="J52" s="8">
         <v>45968.835116782408</v>
       </c>
-      <c r="K52" t="s">
+      <c r="K52" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L52" t="s">
@@ -5875,25 +5960,29 @@
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>18</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="A53" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E53" t="s">
-        <v>20</v>
-      </c>
-      <c r="I53">
+      <c r="D53" s="6"/>
+      <c r="E53" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" s="6"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6">
         <v>4</v>
       </c>
-      <c r="J53" s="2">
+      <c r="J53" s="8">
         <v>45968.835116828697</v>
       </c>
-      <c r="K53" t="s">
+      <c r="K53" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L53" t="s">
@@ -5919,25 +6008,29 @@
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>18</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="A54" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E54" t="s">
-        <v>20</v>
-      </c>
-      <c r="I54">
+      <c r="D54" s="6"/>
+      <c r="E54" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" s="6"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6">
         <v>4</v>
       </c>
-      <c r="J54" s="2">
+      <c r="J54" s="8">
         <v>45968.835117037037</v>
       </c>
-      <c r="K54" t="s">
+      <c r="K54" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L54" t="s">
@@ -5963,25 +6056,29 @@
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>18</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="A55" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E55" t="s">
-        <v>20</v>
-      </c>
-      <c r="I55">
+      <c r="D55" s="6"/>
+      <c r="E55" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" s="6"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6">
         <v>4</v>
       </c>
-      <c r="J55" s="2">
+      <c r="J55" s="8">
         <v>45968.835117071758</v>
       </c>
-      <c r="K55" t="s">
+      <c r="K55" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L55" t="s">
@@ -6007,25 +6104,29 @@
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>18</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="A56" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E56" t="s">
-        <v>20</v>
-      </c>
-      <c r="I56">
+      <c r="D56" s="6"/>
+      <c r="E56" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" s="6"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6">
         <v>3</v>
       </c>
-      <c r="J56" s="2">
+      <c r="J56" s="8">
         <v>45968.835117152783</v>
       </c>
-      <c r="K56" t="s">
+      <c r="K56" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L56" t="s">
@@ -6051,25 +6152,29 @@
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="A57" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E57" t="s">
-        <v>20</v>
-      </c>
-      <c r="I57">
+      <c r="D57" s="6"/>
+      <c r="E57" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F57" s="6"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6">
         <v>11</v>
       </c>
-      <c r="J57" s="2">
+      <c r="J57" s="8">
         <v>45968.835117164352</v>
       </c>
-      <c r="K57" t="s">
+      <c r="K57" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L57" t="s">
@@ -6095,25 +6200,29 @@
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>18</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="A58" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E58" t="s">
-        <v>20</v>
-      </c>
-      <c r="I58">
+      <c r="D58" s="6"/>
+      <c r="E58" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F58" s="6"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6">
         <v>6</v>
       </c>
-      <c r="J58" s="2">
+      <c r="J58" s="8">
         <v>45968.835117268522</v>
       </c>
-      <c r="K58" t="s">
+      <c r="K58" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L58" t="s">
@@ -6139,25 +6248,29 @@
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>18</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="A59" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E59" t="s">
-        <v>20</v>
-      </c>
-      <c r="I59">
+      <c r="D59" s="6"/>
+      <c r="E59" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F59" s="6"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6">
         <v>4</v>
       </c>
-      <c r="J59" s="2">
+      <c r="J59" s="8">
         <v>45968.835117291666</v>
       </c>
-      <c r="K59" t="s">
+      <c r="K59" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L59" t="s">
@@ -6183,25 +6296,29 @@
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>18</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="A60" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E60" t="s">
-        <v>20</v>
-      </c>
-      <c r="I60">
+      <c r="D60" s="6"/>
+      <c r="E60" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F60" s="6"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6">
         <v>21</v>
       </c>
-      <c r="J60" s="2">
+      <c r="J60" s="8">
         <v>45968.835117407412</v>
       </c>
-      <c r="K60" t="s">
+      <c r="K60" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L60" t="s">
@@ -6227,25 +6344,29 @@
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>18</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="A61" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E61" t="s">
-        <v>20</v>
-      </c>
-      <c r="I61">
+      <c r="D61" s="6"/>
+      <c r="E61" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F61" s="6"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6">
         <v>21</v>
       </c>
-      <c r="J61" s="2">
+      <c r="J61" s="8">
         <v>45968.835117407412</v>
       </c>
-      <c r="K61" t="s">
+      <c r="K61" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L61" t="s">
@@ -6271,25 +6392,29 @@
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>18</v>
-      </c>
-      <c r="B62" t="s">
+      <c r="A62" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E62" t="s">
-        <v>20</v>
-      </c>
-      <c r="I62">
+      <c r="D62" s="6"/>
+      <c r="E62" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F62" s="6"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6">
         <v>21</v>
       </c>
-      <c r="J62" s="2">
+      <c r="J62" s="8">
         <v>45968.835117407412</v>
       </c>
-      <c r="K62" t="s">
+      <c r="K62" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L62" t="s">
@@ -6315,25 +6440,29 @@
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>18</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="A63" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E63" t="s">
-        <v>20</v>
-      </c>
-      <c r="I63">
+      <c r="D63" s="6"/>
+      <c r="E63" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F63" s="6"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6">
         <v>21</v>
       </c>
-      <c r="J63" s="2">
+      <c r="J63" s="8">
         <v>45968.835117407412</v>
       </c>
-      <c r="K63" t="s">
+      <c r="K63" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L63" t="s">
@@ -6359,22 +6488,27 @@
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E64" t="s">
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="I64">
+      <c r="G64" s="7"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6">
         <v>21</v>
       </c>
-      <c r="J64" s="2">
+      <c r="J64" s="8">
         <v>45968.835117407412</v>
       </c>
-      <c r="K64" t="s">
+      <c r="K64" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L64" t="s">
@@ -6397,25 +6531,29 @@
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E65" t="s">
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="G65" s="3" t="s">
+      <c r="G65" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="I65">
+      <c r="H65" s="6"/>
+      <c r="I65" s="6">
         <v>21</v>
       </c>
-      <c r="J65" s="2">
+      <c r="J65" s="8">
         <v>45968.835117407412</v>
       </c>
-      <c r="K65" t="s">
+      <c r="K65" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L65" t="s">
@@ -6438,25 +6576,29 @@
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A66" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E66" t="s">
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="G66" s="3" t="s">
+      <c r="G66" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="I66">
+      <c r="H66" s="6"/>
+      <c r="I66" s="6">
         <v>21</v>
       </c>
-      <c r="J66" s="2">
+      <c r="J66" s="8">
         <v>45968.835117407412</v>
       </c>
-      <c r="K66" t="s">
+      <c r="K66" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L66" t="s">
@@ -6479,25 +6621,29 @@
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="A67" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E67" t="s">
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="G67" s="3" t="s">
+      <c r="G67" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="I67">
+      <c r="H67" s="6"/>
+      <c r="I67" s="6">
         <v>21</v>
       </c>
-      <c r="J67" s="2">
+      <c r="J67" s="8">
         <v>45968.835117407412</v>
       </c>
-      <c r="K67" t="s">
+      <c r="K67" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L67" t="s">
@@ -6520,25 +6666,29 @@
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>18</v>
-      </c>
-      <c r="B68" t="s">
+      <c r="A68" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E68" t="s">
-        <v>20</v>
-      </c>
-      <c r="I68">
+      <c r="D68" s="6"/>
+      <c r="E68" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F68" s="6"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6">
         <v>19</v>
       </c>
-      <c r="J68" s="2">
+      <c r="J68" s="8">
         <v>45968.835117476847</v>
       </c>
-      <c r="K68" t="s">
+      <c r="K68" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L68" t="s">
@@ -6564,22 +6714,27 @@
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E69" t="s">
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="I69">
+      <c r="G69" s="7"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6">
         <v>19</v>
       </c>
-      <c r="J69" s="2">
+      <c r="J69" s="8">
         <v>45968.835117476847</v>
       </c>
-      <c r="K69" t="s">
+      <c r="K69" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L69" t="s">
@@ -6602,25 +6757,29 @@
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E70" t="s">
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="G70" s="3" t="s">
+      <c r="G70" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="I70">
+      <c r="H70" s="6"/>
+      <c r="I70" s="6">
         <v>19</v>
       </c>
-      <c r="J70" s="2">
+      <c r="J70" s="8">
         <v>45968.835117476847</v>
       </c>
-      <c r="K70" t="s">
+      <c r="K70" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L70" t="s">
@@ -6643,25 +6802,29 @@
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>18</v>
-      </c>
-      <c r="B71" t="s">
+      <c r="A71" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E71" t="s">
-        <v>20</v>
-      </c>
-      <c r="I71">
+      <c r="D71" s="6"/>
+      <c r="E71" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F71" s="6"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6">
         <v>6</v>
       </c>
-      <c r="J71" s="2">
+      <c r="J71" s="8">
         <v>45968.83511763889</v>
       </c>
-      <c r="K71" t="s">
+      <c r="K71" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L71" t="s">
@@ -6687,25 +6850,29 @@
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>18</v>
-      </c>
-      <c r="B72" t="s">
+      <c r="A72" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E72" t="s">
-        <v>20</v>
-      </c>
-      <c r="I72">
+      <c r="D72" s="6"/>
+      <c r="E72" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F72" s="6"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6">
         <v>3</v>
       </c>
-      <c r="J72" s="2">
+      <c r="J72" s="8">
         <v>45968.83511763889</v>
       </c>
-      <c r="K72" t="s">
+      <c r="K72" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L72" t="s">
@@ -6731,25 +6898,29 @@
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>18</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="A73" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B73" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E73" t="s">
-        <v>20</v>
-      </c>
-      <c r="I73">
+      <c r="D73" s="6"/>
+      <c r="E73" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73" s="6"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6">
         <v>5</v>
       </c>
-      <c r="J73" s="2">
+      <c r="J73" s="8">
         <v>45968.83511763889</v>
       </c>
-      <c r="K73" t="s">
+      <c r="K73" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L73" t="s">
@@ -6775,25 +6946,29 @@
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E74" t="s">
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F74" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="H74" t="s">
+      <c r="G74" s="7"/>
+      <c r="H74" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="I74">
+      <c r="I74" s="6">
         <v>39</v>
       </c>
-      <c r="J74" s="2">
+      <c r="J74" s="8">
         <v>45968.835117719907</v>
       </c>
-      <c r="K74" t="s">
+      <c r="K74" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L74" t="s">
@@ -6816,25 +6991,29 @@
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>18</v>
-      </c>
-      <c r="B75" t="s">
+      <c r="A75" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B75" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E75" t="s">
-        <v>20</v>
-      </c>
-      <c r="I75">
+      <c r="D75" s="6"/>
+      <c r="E75" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F75" s="6"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6">
         <v>39</v>
       </c>
-      <c r="J75" s="2">
+      <c r="J75" s="8">
         <v>45968.835117719907</v>
       </c>
-      <c r="K75" t="s">
+      <c r="K75" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L75" t="s">
@@ -6860,25 +7039,29 @@
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>18</v>
-      </c>
-      <c r="B76" t="s">
+      <c r="A76" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B76" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E76" t="s">
-        <v>20</v>
-      </c>
-      <c r="I76">
+      <c r="D76" s="6"/>
+      <c r="E76" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76" s="6"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6">
         <v>39</v>
       </c>
-      <c r="J76" s="2">
+      <c r="J76" s="8">
         <v>45968.835117719907</v>
       </c>
-      <c r="K76" t="s">
+      <c r="K76" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L76" t="s">
@@ -6904,25 +7087,29 @@
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>18</v>
-      </c>
-      <c r="B77" t="s">
+      <c r="A77" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B77" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E77" t="s">
-        <v>20</v>
-      </c>
-      <c r="I77">
+      <c r="D77" s="6"/>
+      <c r="E77" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F77" s="6"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6">
         <v>39</v>
       </c>
-      <c r="J77" s="2">
+      <c r="J77" s="8">
         <v>45968.835117719907</v>
       </c>
-      <c r="K77" t="s">
+      <c r="K77" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L77" t="s">
@@ -6948,25 +7135,29 @@
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>18</v>
-      </c>
-      <c r="B78" t="s">
+      <c r="A78" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B78" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E78" t="s">
-        <v>20</v>
-      </c>
-      <c r="I78">
+      <c r="D78" s="6"/>
+      <c r="E78" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F78" s="6"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6">
         <v>14</v>
       </c>
-      <c r="J78" s="2">
+      <c r="J78" s="8">
         <v>45968.835117939823</v>
       </c>
-      <c r="K78" t="s">
+      <c r="K78" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L78" t="s">
@@ -6992,25 +7183,29 @@
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>18</v>
-      </c>
-      <c r="B79" t="s">
+      <c r="A79" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="E79" t="s">
-        <v>20</v>
-      </c>
-      <c r="I79">
+      <c r="D79" s="6"/>
+      <c r="E79" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79" s="6"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6">
         <v>6</v>
       </c>
-      <c r="J79" s="2">
+      <c r="J79" s="8">
         <v>45968.835117997682</v>
       </c>
-      <c r="K79" t="s">
+      <c r="K79" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L79" t="s">
@@ -7036,25 +7231,29 @@
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>18</v>
-      </c>
-      <c r="B80" t="s">
+      <c r="A80" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E80" t="s">
-        <v>20</v>
-      </c>
-      <c r="I80">
+      <c r="D80" s="6"/>
+      <c r="E80" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F80" s="6"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6">
         <v>6</v>
       </c>
-      <c r="J80" s="2">
+      <c r="J80" s="8">
         <v>45968.835117997682</v>
       </c>
-      <c r="K80" t="s">
+      <c r="K80" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L80" t="s">
@@ -7080,25 +7279,29 @@
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="A81" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E81" t="s">
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G81" s="3" t="s">
+      <c r="G81" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="I81">
+      <c r="H81" s="6"/>
+      <c r="I81" s="6">
         <v>29</v>
       </c>
-      <c r="J81" s="2">
+      <c r="J81" s="8">
         <v>45968.835118055547</v>
       </c>
-      <c r="K81" t="s">
+      <c r="K81" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L81" t="s">
@@ -7121,25 +7324,29 @@
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="A82" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E82" t="s">
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="G82" s="3" t="s">
+      <c r="G82" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="I82">
+      <c r="H82" s="6"/>
+      <c r="I82" s="6">
         <v>29</v>
       </c>
-      <c r="J82" s="2">
+      <c r="J82" s="8">
         <v>45968.835118055547</v>
       </c>
-      <c r="K82" t="s">
+      <c r="K82" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L82" t="s">
@@ -7162,22 +7369,27 @@
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="A83" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E83" t="s">
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="I83">
+      <c r="G83" s="7"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6">
         <v>29</v>
       </c>
-      <c r="J83" s="2">
+      <c r="J83" s="8">
         <v>45968.835118055547</v>
       </c>
-      <c r="K83" t="s">
+      <c r="K83" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L83" t="s">
@@ -7200,25 +7412,29 @@
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>18</v>
-      </c>
-      <c r="B84" t="s">
+      <c r="A84" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B84" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="E84" t="s">
-        <v>20</v>
-      </c>
-      <c r="I84">
+      <c r="D84" s="6"/>
+      <c r="E84" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F84" s="6"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6">
         <v>10</v>
       </c>
-      <c r="J84" s="2">
+      <c r="J84" s="8">
         <v>45968.835118194453</v>
       </c>
-      <c r="K84" t="s">
+      <c r="K84" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L84" t="s">
@@ -7244,25 +7460,29 @@
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>18</v>
-      </c>
-      <c r="B85" t="s">
+      <c r="A85" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B85" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E85" t="s">
-        <v>20</v>
-      </c>
-      <c r="I85">
+      <c r="D85" s="6"/>
+      <c r="E85" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F85" s="6"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6">
         <v>10</v>
       </c>
-      <c r="J85" s="2">
+      <c r="J85" s="8">
         <v>45968.835118194453</v>
       </c>
-      <c r="K85" t="s">
+      <c r="K85" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L85" t="s">
@@ -7288,25 +7508,29 @@
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="A86" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E86" t="s">
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="G86" s="3" t="s">
+      <c r="G86" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="I86">
+      <c r="H86" s="6"/>
+      <c r="I86" s="6">
         <v>10</v>
       </c>
-      <c r="J86" s="2">
+      <c r="J86" s="8">
         <v>45968.835118194453</v>
       </c>
-      <c r="K86" t="s">
+      <c r="K86" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L86" t="s">
@@ -7329,25 +7553,29 @@
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>18</v>
-      </c>
-      <c r="B87" t="s">
+      <c r="A87" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B87" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="E87" t="s">
-        <v>20</v>
-      </c>
-      <c r="I87">
+      <c r="D87" s="6"/>
+      <c r="E87" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F87" s="6"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6">
         <v>4</v>
       </c>
-      <c r="J87" s="2">
+      <c r="J87" s="8">
         <v>45968.835118194453</v>
       </c>
-      <c r="K87" t="s">
+      <c r="K87" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L87" t="s">
@@ -7373,25 +7601,29 @@
       </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>18</v>
-      </c>
-      <c r="B88" t="s">
+      <c r="A88" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B88" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E88" t="s">
-        <v>20</v>
-      </c>
-      <c r="I88">
+      <c r="D88" s="6"/>
+      <c r="E88" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F88" s="6"/>
+      <c r="G88" s="7"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6">
         <v>4</v>
       </c>
-      <c r="J88" s="2">
+      <c r="J88" s="8">
         <v>45968.835118298608</v>
       </c>
-      <c r="K88" t="s">
+      <c r="K88" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L88" t="s">
@@ -7417,25 +7649,29 @@
       </c>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>18</v>
-      </c>
-      <c r="B89" t="s">
+      <c r="A89" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B89" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="E89" t="s">
-        <v>20</v>
-      </c>
-      <c r="I89">
+      <c r="D89" s="6"/>
+      <c r="E89" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F89" s="6"/>
+      <c r="G89" s="7"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6">
         <v>6</v>
       </c>
-      <c r="J89" s="2">
+      <c r="J89" s="8">
         <v>45968.835118368057</v>
       </c>
-      <c r="K89" t="s">
+      <c r="K89" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L89" t="s">
@@ -7461,25 +7697,29 @@
       </c>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>18</v>
-      </c>
-      <c r="B90" t="s">
+      <c r="A90" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B90" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="E90" t="s">
-        <v>20</v>
-      </c>
-      <c r="I90">
+      <c r="D90" s="6"/>
+      <c r="E90" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F90" s="6"/>
+      <c r="G90" s="7"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6">
         <v>15</v>
       </c>
-      <c r="J90" s="2">
+      <c r="J90" s="8">
         <v>45968.835118402778</v>
       </c>
-      <c r="K90" t="s">
+      <c r="K90" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L90" t="s">
@@ -7505,25 +7745,29 @@
       </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>18</v>
-      </c>
-      <c r="B91" t="s">
+      <c r="A91" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B91" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E91" t="s">
-        <v>20</v>
-      </c>
-      <c r="I91">
+      <c r="D91" s="6"/>
+      <c r="E91" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F91" s="6"/>
+      <c r="G91" s="7"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6">
         <v>2</v>
       </c>
-      <c r="J91" s="2">
+      <c r="J91" s="8">
         <v>45968.835118518517</v>
       </c>
-      <c r="K91" t="s">
+      <c r="K91" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L91" t="s">
@@ -7549,25 +7793,29 @@
       </c>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>18</v>
-      </c>
-      <c r="B92" t="s">
+      <c r="A92" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B92" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="E92" t="s">
-        <v>20</v>
-      </c>
-      <c r="I92">
+      <c r="D92" s="6"/>
+      <c r="E92" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F92" s="6"/>
+      <c r="G92" s="7"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6">
         <v>2</v>
       </c>
-      <c r="J92" s="2">
+      <c r="J92" s="8">
         <v>45968.835118518517</v>
       </c>
-      <c r="K92" t="s">
+      <c r="K92" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L92" t="s">
@@ -7593,25 +7841,29 @@
       </c>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>18</v>
-      </c>
-      <c r="B93" t="s">
+      <c r="A93" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B93" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="E93" t="s">
-        <v>20</v>
-      </c>
-      <c r="I93">
+      <c r="D93" s="6"/>
+      <c r="E93" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F93" s="6"/>
+      <c r="G93" s="7"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6">
         <v>11</v>
       </c>
-      <c r="J93" s="2">
+      <c r="J93" s="8">
         <v>45968.835118553237</v>
       </c>
-      <c r="K93" t="s">
+      <c r="K93" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L93" t="s">
@@ -7637,25 +7889,29 @@
       </c>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>18</v>
-      </c>
-      <c r="B94" t="s">
+      <c r="A94" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B94" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E94" t="s">
-        <v>20</v>
-      </c>
-      <c r="I94">
+      <c r="D94" s="6"/>
+      <c r="E94" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F94" s="6"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6">
         <v>11</v>
       </c>
-      <c r="J94" s="2">
+      <c r="J94" s="8">
         <v>45968.835118553237</v>
       </c>
-      <c r="K94" t="s">
+      <c r="K94" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L94" t="s">
@@ -7681,25 +7937,29 @@
       </c>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>18</v>
-      </c>
-      <c r="B95" t="s">
+      <c r="A95" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B95" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="E95" t="s">
-        <v>20</v>
-      </c>
-      <c r="I95">
+      <c r="D95" s="6"/>
+      <c r="E95" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F95" s="6"/>
+      <c r="G95" s="7"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6">
         <v>45</v>
       </c>
-      <c r="J95" s="2">
+      <c r="J95" s="8">
         <v>45968.83511861111</v>
       </c>
-      <c r="K95" t="s">
+      <c r="K95" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L95" t="s">
@@ -7725,25 +7985,29 @@
       </c>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>18</v>
-      </c>
-      <c r="B96" t="s">
+      <c r="A96" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B96" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="E96" t="s">
-        <v>20</v>
-      </c>
-      <c r="I96">
+      <c r="D96" s="6"/>
+      <c r="E96" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F96" s="6"/>
+      <c r="G96" s="7"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6">
         <v>45</v>
       </c>
-      <c r="J96" s="2">
+      <c r="J96" s="8">
         <v>45968.83511861111</v>
       </c>
-      <c r="K96" t="s">
+      <c r="K96" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L96" t="s">
@@ -7769,25 +8033,29 @@
       </c>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>18</v>
-      </c>
-      <c r="B97" t="s">
+      <c r="A97" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B97" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="E97" t="s">
-        <v>20</v>
-      </c>
-      <c r="I97">
+      <c r="D97" s="6"/>
+      <c r="E97" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F97" s="6"/>
+      <c r="G97" s="7"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6">
         <v>45</v>
       </c>
-      <c r="J97" s="2">
+      <c r="J97" s="8">
         <v>45968.83511861111</v>
       </c>
-      <c r="K97" t="s">
+      <c r="K97" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L97" t="s">
@@ -7813,25 +8081,29 @@
       </c>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>18</v>
-      </c>
-      <c r="B98" t="s">
+      <c r="A98" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B98" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="E98" t="s">
-        <v>20</v>
-      </c>
-      <c r="I98">
+      <c r="D98" s="6"/>
+      <c r="E98" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F98" s="6"/>
+      <c r="G98" s="7"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6">
         <v>47</v>
       </c>
-      <c r="J98" s="2">
+      <c r="J98" s="8">
         <v>45968.835118680552</v>
       </c>
-      <c r="K98" t="s">
+      <c r="K98" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L98" t="s">
@@ -7857,25 +8129,29 @@
       </c>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>18</v>
-      </c>
-      <c r="B99" t="s">
+      <c r="A99" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B99" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E99" t="s">
-        <v>20</v>
-      </c>
-      <c r="I99">
+      <c r="D99" s="6"/>
+      <c r="E99" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F99" s="6"/>
+      <c r="G99" s="7"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6">
         <v>10</v>
       </c>
-      <c r="J99" s="2">
+      <c r="J99" s="8">
         <v>45968.835118750001</v>
       </c>
-      <c r="K99" t="s">
+      <c r="K99" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L99" t="s">
@@ -7901,25 +8177,29 @@
       </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="A100" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E100" t="s">
+      <c r="B100" s="6"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F100" t="s">
+      <c r="F100" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="G100" s="3" t="s">
+      <c r="G100" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="I100">
+      <c r="H100" s="6"/>
+      <c r="I100" s="6">
         <v>10</v>
       </c>
-      <c r="J100" s="2">
+      <c r="J100" s="8">
         <v>45968.835118750001</v>
       </c>
-      <c r="K100" t="s">
+      <c r="K100" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L100" t="s">
@@ -7942,22 +8222,27 @@
       </c>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>18</v>
-      </c>
-      <c r="B101" t="s">
+      <c r="A101" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B101" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="E101" t="s">
-        <v>20</v>
-      </c>
-      <c r="I101">
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F101" s="6"/>
+      <c r="G101" s="7"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6">
         <v>3</v>
       </c>
-      <c r="J101" s="2">
+      <c r="J101" s="8">
         <v>45968.835118854156</v>
       </c>
-      <c r="K101" t="s">
+      <c r="K101" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L101" t="s">
@@ -7983,25 +8268,29 @@
       </c>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>18</v>
-      </c>
-      <c r="B102" t="s">
+      <c r="A102" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B102" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E102" t="s">
-        <v>20</v>
-      </c>
-      <c r="I102">
+      <c r="D102" s="6"/>
+      <c r="E102" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F102" s="6"/>
+      <c r="G102" s="7"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6">
         <v>15</v>
       </c>
-      <c r="J102" s="2">
+      <c r="J102" s="8">
         <v>45968.835118958334</v>
       </c>
-      <c r="K102" t="s">
+      <c r="K102" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L102" t="s">
@@ -8027,25 +8316,29 @@
       </c>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>18</v>
-      </c>
-      <c r="B103" t="s">
+      <c r="A103" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B103" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E103" t="s">
-        <v>20</v>
-      </c>
-      <c r="I103">
+      <c r="D103" s="6"/>
+      <c r="E103" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F103" s="6"/>
+      <c r="G103" s="7"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6">
         <v>10</v>
       </c>
-      <c r="J103" s="2">
+      <c r="J103" s="8">
         <v>45968.835119143521</v>
       </c>
-      <c r="K103" t="s">
+      <c r="K103" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L103" t="s">
@@ -8071,25 +8364,29 @@
       </c>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>18</v>
-      </c>
-      <c r="B104" t="s">
+      <c r="A104" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B104" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E104" t="s">
-        <v>20</v>
-      </c>
-      <c r="I104">
+      <c r="D104" s="6"/>
+      <c r="E104" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F104" s="6"/>
+      <c r="G104" s="7"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6">
         <v>31</v>
       </c>
-      <c r="J104" s="2">
+      <c r="J104" s="8">
         <v>45968.835119212963</v>
       </c>
-      <c r="K104" t="s">
+      <c r="K104" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L104" t="s">
@@ -8115,25 +8412,29 @@
       </c>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>18</v>
-      </c>
-      <c r="B105" t="s">
+      <c r="A105" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B105" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="E105" t="s">
-        <v>20</v>
-      </c>
-      <c r="I105">
+      <c r="D105" s="6"/>
+      <c r="E105" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F105" s="6"/>
+      <c r="G105" s="7"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6">
         <v>31</v>
       </c>
-      <c r="J105" s="2">
+      <c r="J105" s="8">
         <v>45968.835119212963</v>
       </c>
-      <c r="K105" t="s">
+      <c r="K105" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L105" t="s">
@@ -8159,25 +8460,29 @@
       </c>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>18</v>
-      </c>
-      <c r="B106" t="s">
+      <c r="A106" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B106" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E106" t="s">
-        <v>20</v>
-      </c>
-      <c r="I106">
+      <c r="D106" s="6"/>
+      <c r="E106" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F106" s="6"/>
+      <c r="G106" s="7"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6">
         <v>31</v>
       </c>
-      <c r="J106" s="2">
+      <c r="J106" s="8">
         <v>45968.835119212963</v>
       </c>
-      <c r="K106" t="s">
+      <c r="K106" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L106" t="s">
@@ -8203,22 +8508,27 @@
       </c>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="A107" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E107" t="s">
+      <c r="B107" s="6"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F107" t="s">
+      <c r="F107" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="I107">
+      <c r="G107" s="7"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6">
         <v>31</v>
       </c>
-      <c r="J107" s="2">
+      <c r="J107" s="8">
         <v>45968.835119212963</v>
       </c>
-      <c r="K107" t="s">
+      <c r="K107" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L107" t="s">
@@ -8241,25 +8551,29 @@
       </c>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>18</v>
-      </c>
-      <c r="B108" t="s">
+      <c r="A108" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B108" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="E108" t="s">
-        <v>20</v>
-      </c>
-      <c r="I108">
+      <c r="D108" s="6"/>
+      <c r="E108" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F108" s="6"/>
+      <c r="G108" s="7"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6">
         <v>3</v>
       </c>
-      <c r="J108" s="2">
+      <c r="J108" s="8">
         <v>45968.835119305557</v>
       </c>
-      <c r="K108" t="s">
+      <c r="K108" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L108" t="s">
@@ -8285,25 +8599,29 @@
       </c>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>18</v>
-      </c>
-      <c r="B109" t="s">
+      <c r="A109" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B109" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="E109" t="s">
-        <v>20</v>
-      </c>
-      <c r="I109">
+      <c r="D109" s="6"/>
+      <c r="E109" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F109" s="6"/>
+      <c r="G109" s="7"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="6">
         <v>44</v>
       </c>
-      <c r="J109" s="2">
+      <c r="J109" s="8">
         <v>45968.835119502313</v>
       </c>
-      <c r="K109" t="s">
+      <c r="K109" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L109" t="s">
@@ -8329,25 +8647,29 @@
       </c>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="A110" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E110" t="s">
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F110" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="G110" s="3" t="s">
+      <c r="G110" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="I110">
+      <c r="H110" s="6"/>
+      <c r="I110" s="6">
         <v>44</v>
       </c>
-      <c r="J110" s="2">
+      <c r="J110" s="8">
         <v>45968.835119502313</v>
       </c>
-      <c r="K110" t="s">
+      <c r="K110" s="6" t="s">
         <v>58</v>
       </c>
       <c r="L110" t="s">

</xml_diff>